<commit_message>
time out . task
</commit_message>
<xml_diff>
--- a/ExcelConfig/battleLevel.xlsx
+++ b/ExcelConfig/battleLevel.xlsx
@@ -13,8 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="__Base" sheetId="2" r:id="rId1"/>
-    <sheet name="MonsterData" sheetId="6" r:id="rId2"/>
-    <sheet name="BattleLevelData" sheetId="1" r:id="rId3"/>
+    <sheet name="BattleLevelData" sheetId="1" r:id="rId2"/>
+    <sheet name="MonsterData" sheetId="6" r:id="rId3"/>
     <sheet name="MonsterGroupData" sheetId="3" r:id="rId4"/>
     <sheet name="DropGroupData" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -657,6 +657,20 @@
   </si>
   <si>
     <t>1|1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxPlayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大玩家数</t>
+    <rPh sb="0" eb="1">
+      <t>zui da</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>wan jia shu</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1186,11 +1200,169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:R2">
+      <formula1>"String,Int,DateTime,Float"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1447,151 +1619,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:Q2">
-      <formula1>"String,Int,DateTime,Float"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>